<commit_message>
COMMIT 02 : MODULE 1.3
Suivi, Gantt, Tableau de tests, Processing, Arduino
</commit_message>
<xml_diff>
--- a/Fiche de suivi.xlsx
+++ b/Fiche de suivi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31615DC2-0E0B-44BB-B1EC-F36772DC8FA1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62FC39C-156F-43B0-9806-243B59B1A66F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,6 +564,9 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="2">
+        <v>0.3576388888888889</v>
+      </c>
       <c r="K3" t="s">
         <v>3</v>
       </c>
@@ -590,6 +593,9 @@
       <c r="F4" t="s">
         <v>4</v>
       </c>
+      <c r="G4" s="2">
+        <v>0.32291666666666669</v>
+      </c>
       <c r="K4" t="s">
         <v>4</v>
       </c>
@@ -616,6 +622,9 @@
       <c r="F5" t="s">
         <v>5</v>
       </c>
+      <c r="G5" s="2">
+        <v>0.34722222222222227</v>
+      </c>
       <c r="K5" t="s">
         <v>5</v>
       </c>
@@ -641,6 +650,9 @@
       </c>
       <c r="F6" t="s">
         <v>6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.3576388888888889</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
COMMIT 02 : [Mathis] (Suivi)
</commit_message>
<xml_diff>
--- a/Fiche de suivi.xlsx
+++ b/Fiche de suivi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62FC39C-156F-43B0-9806-243B59B1A66F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D626F6-2983-4394-B655-B200C3AE7ABD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>Heure d'arrivée</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>Membres</t>
+  </si>
+  <si>
+    <t>Schéma électrique, début du programme Arduino</t>
+  </si>
+  <si>
+    <t>Programme en C</t>
+  </si>
+  <si>
+    <t>Gantt, Trello, Rapport, Tests sur Processing + Arduino</t>
+  </si>
+  <si>
+    <t>Continue le programme C (Structures, commentaires, nombre de lignes en mémoire)</t>
   </si>
 </sst>
 </file>
@@ -443,7 +455,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,7 +467,7 @@
     <col min="6" max="6" width="21.109375" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="9" max="9" width="68.33203125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
     <col min="12" max="12" width="16.77734375" customWidth="1"/>
     <col min="13" max="14" width="17.109375" customWidth="1"/>
@@ -567,6 +579,12 @@
       <c r="G3" s="2">
         <v>0.3576388888888889</v>
       </c>
+      <c r="H3" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
       <c r="K3" t="s">
         <v>3</v>
       </c>
@@ -596,6 +614,12 @@
       <c r="G4" s="2">
         <v>0.32291666666666669</v>
       </c>
+      <c r="H4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
       <c r="K4" t="s">
         <v>4</v>
       </c>
@@ -625,6 +649,12 @@
       <c r="G5" s="2">
         <v>0.34722222222222227</v>
       </c>
+      <c r="H5" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
       <c r="K5" t="s">
         <v>5</v>
       </c>
@@ -653,6 +683,12 @@
       </c>
       <c r="G6" s="2">
         <v>0.3576388888888889</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>

</xml_diff>